<commit_message>
Updated theme to red/white, README.md; Added footer with reference to logos
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
@@ -2456,7 +2456,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="EEA1" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9F66" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2537,7 +2537,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="C534" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="886B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -2744,7 +2744,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E351" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="D0EE" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -2820,7 +2820,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="949B" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A84D" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -2942,7 +2942,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D458" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A84F" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3094,7 +3094,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A504" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="86D4" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3304,7 +3304,7 @@
       <c r="P4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B372" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E3DE" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:P4"/>
   </mergeCells>
@@ -3473,7 +3473,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B8BB" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="FCA4" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3600,7 +3600,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="ABA0" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E61C" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4389,7 +4389,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9728" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A146" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4478,7 +4478,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A9D9" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="AF65" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -4633,7 +4633,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A13A" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="880D" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -4826,7 +4826,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="F43E" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E731" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5195,7 +5195,7 @@
       <c r="AD4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D3D1" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9221" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:AD4"/>
   </mergeCells>
@@ -5414,7 +5414,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="CD33" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="EB68" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Prevent scrollbar from appearing underneath navbar
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
@@ -2456,7 +2456,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="9F66" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="DBA0" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2537,7 +2537,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="886B" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="812E" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -2744,7 +2744,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D0EE" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="AF2B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -2820,7 +2820,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A84D" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F3EA" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -2942,7 +2942,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A84F" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="DE82" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3094,7 +3094,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="86D4" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C58C" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3304,7 +3304,7 @@
       <c r="P4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E3DE" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="BD55" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:P4"/>
   </mergeCells>
@@ -3473,7 +3473,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="FCA4" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9032" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3600,7 +3600,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E61C" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F601" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4389,7 +4389,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A146" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="BC96" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4478,7 +4478,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="AF65" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9C95" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -4633,7 +4633,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="880D" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E5CA" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -4826,7 +4826,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E731" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9600" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5195,7 +5195,7 @@
       <c r="AD4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9221" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B335" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:AD4"/>
   </mergeCells>
@@ -5414,7 +5414,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="EB68" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="FAB4" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Removed references to '.css.map' files
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
@@ -2456,7 +2456,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="8A9C" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="80D2" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2537,7 +2537,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A71B" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B0B6" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -2744,7 +2744,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="98E6" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C7D6" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -2820,7 +2820,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="81EF" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="838A" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -2942,7 +2942,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="EC3A" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E13A" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3094,7 +3094,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A1FE" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E25E" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3304,7 +3304,7 @@
       <c r="P4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D5E5" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="8410" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:P4"/>
   </mergeCells>
@@ -3473,7 +3473,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B762" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="AAFC" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3600,7 +3600,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="C35A" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="AFD9" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4389,7 +4389,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9FF8" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="8D54" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4478,7 +4478,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="DDB7" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9B4E" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -4633,7 +4633,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E701" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="FBD9" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -4826,7 +4826,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="CCFA" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="AFC2" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5195,7 +5195,7 @@
       <c r="AD4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="954A" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="92BC" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:AD4"/>
   </mergeCells>
@@ -5414,7 +5414,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="F15A" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="FE72" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Removed field reference; Added has  search
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
@@ -2456,7 +2456,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="EFD2" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E2B4" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2537,7 +2537,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E727" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="BCCC" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -2744,7 +2744,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D7C8" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="CE0C" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -2820,7 +2820,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="FEB3" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="AB58" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -2942,7 +2942,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="F506" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="BCE3" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3094,7 +3094,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="AD27" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B8C7" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3304,7 +3304,7 @@
       <c r="P4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E2D3" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A552" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:P4"/>
   </mergeCells>
@@ -3473,7 +3473,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9095" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="878F" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3600,7 +3600,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B922" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="96AD" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4389,7 +4389,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="BB3F" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="8320" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4478,7 +4478,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D8AC" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="809C" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -4633,7 +4633,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E3BE" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E5AE" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -4826,7 +4826,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A358" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9069" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5195,7 +5195,7 @@
       <c r="AD4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="8C39" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="8419" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:AD4"/>
   </mergeCells>
@@ -5414,7 +5414,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D88F" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F6B5" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Replaced copyright reference with licence reference in footer; Added "noopener noreferrer" for external links;
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
@@ -2456,7 +2456,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="C558" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C3D8" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2537,7 +2537,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="FA27" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B2C0" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -2744,7 +2744,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D13A" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C5B4" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -2820,7 +2820,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E680" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="EFE6" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -2942,7 +2942,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D856" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="D6F8" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3094,7 +3094,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="F179" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="FB31" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3304,7 +3304,7 @@
       <c r="P4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="85AE" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="D46B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:P4"/>
   </mergeCells>
@@ -3473,7 +3473,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="F6CE" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="BA21" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3600,7 +3600,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D5F4" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A0B0" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4389,7 +4389,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E331" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B66C" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4478,7 +4478,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D08B" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="DBF9" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -4633,7 +4633,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="CA96" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A504" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -4826,7 +4826,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D064" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B1E4" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5195,7 +5195,7 @@
       <c r="AD4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="F232" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="EDB2" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:AD4"/>
   </mergeCells>
@@ -5414,7 +5414,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E813" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="D161" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Changed to tiled background; Renamed file names; Changed COPO logo to fully white
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
@@ -2456,7 +2456,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="C3D8" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9DB0" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2537,7 +2537,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B2C0" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A8FC" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -2744,7 +2744,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="C5B4" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9867" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -2820,7 +2820,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="EFE6" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C0C3" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -2942,7 +2942,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D6F8" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="FC72" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3094,7 +3094,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="FB31" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E9C9" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3304,7 +3304,7 @@
       <c r="P4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D46B" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="EFE8" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:P4"/>
   </mergeCells>
@@ -3473,7 +3473,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="BA21" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="ADCB" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3600,7 +3600,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A0B0" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="DF26" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4389,7 +4389,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B66C" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="BB0B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4478,7 +4478,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="DBF9" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="FBD5" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -4633,7 +4633,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A504" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C7EE" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -4826,7 +4826,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B1E4" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A343" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5195,7 +5195,7 @@
       <c r="AD4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="EDB2" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9782" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:AD4"/>
   </mergeCells>
@@ -5414,7 +5414,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D161" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="ABE3" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Added same reference identity terms; Fixed scroll to term
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.3.xlsx
@@ -2456,7 +2456,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="9DB0" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A0F7" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2537,7 +2537,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A8FC" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="918B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -2744,7 +2744,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9867" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="8829" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -2820,7 +2820,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="C0C3" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B6B1" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -2942,7 +2942,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="FC72" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A530" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3094,7 +3094,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E9C9" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A78A" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3304,7 +3304,7 @@
       <c r="P4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="EFE8" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="DBD3" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:P4"/>
   </mergeCells>
@@ -3473,7 +3473,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="ADCB" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B84B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -3600,7 +3600,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="DF26" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C0AE" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4389,7 +4389,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="BB0B" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A92E" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4478,7 +4478,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="FBD5" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C8BF" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -4633,7 +4633,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="C7EE" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9FE4" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -4826,7 +4826,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A343" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F9D6" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5195,7 +5195,7 @@
       <c r="AD4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9782" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="8B28" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:AD4"/>
   </mergeCells>
@@ -5414,7 +5414,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="ABE3" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="DDF8" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>